<commit_message>
added f vs GW data trends for rotor hubs
</commit_message>
<xml_diff>
--- a/docs/flat_plate_drag/flat_plate_drag_data.xlsx
+++ b/docs/flat_plate_drag/flat_plate_drag_data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfiyandyhr/Github_Repos/MCEVS/docs/flat_plate_drag/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A3565B0-94A3-C84E-A60F-02787E7D997E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FE4D78-4895-4D4B-9519-2BA82FB7B666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15320" yWindow="740" windowWidth="14920" windowHeight="18900" activeTab="1" xr2:uid="{9B207304-6C5B-A545-A29F-FC1BAC0A7ED9}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" xr2:uid="{9B207304-6C5B-A545-A29F-FC1BAC0A7ED9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="fuselage" sheetId="1" r:id="rId1"/>
+    <sheet name="hub" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="87">
   <si>
     <t>No</t>
   </si>
@@ -318,6 +319,9 @@
   <si>
     <t>EPFD induced</t>
   </si>
+  <si>
+    <t>With fairing</t>
+  </si>
 </sst>
 </file>
 
@@ -326,7 +330,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -354,6 +358,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -375,7 +385,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -480,11 +490,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -573,6 +603,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -650,7 +707,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$F$5:$F$83</c:f>
+              <c:f>fuselage!$F$5:$F$83</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="79"/>
@@ -896,7 +953,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$5:$E$83</c:f>
+              <c:f>fuselage!$E$5:$E$83</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="79"/>
@@ -1187,7 +1244,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$L$3:$L$21</c:f>
+              <c:f>fuselage!$L$3:$L$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -1253,7 +1310,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$M$3:$M$21</c:f>
+              <c:f>fuselage!$M$3:$M$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -1364,7 +1421,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$I$3:$I$21</c:f>
+              <c:f>fuselage!$I$3:$I$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -1430,7 +1487,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$J$3:$J$21</c:f>
+              <c:f>fuselage!$J$3:$J$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -1532,7 +1589,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$F$3:$F$4</c:f>
+              <c:f>fuselage!$F$3:$F$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1547,7 +1604,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$4</c:f>
+              <c:f>fuselage!$E$3:$E$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1607,7 +1664,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$O$3:$O$23</c:f>
+              <c:f>fuselage!$O$3:$O$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -1679,7 +1736,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$P$3:$P$23</c:f>
+              <c:f>fuselage!$P$3:$P$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -1830,7 +1887,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$F$84:$F$96</c:f>
+              <c:f>fuselage!$F$84:$F$96</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1878,7 +1935,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$84:$E$96</c:f>
+              <c:f>fuselage!$E$84:$E$96</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1959,7 +2016,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$F$97:$F$98</c:f>
+              <c:f>fuselage!$F$97:$F$98</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1974,7 +2031,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$97:$E$98</c:f>
+              <c:f>fuselage!$E$97:$E$98</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="2"/>
@@ -2034,7 +2091,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$R$3:$R$23</c:f>
+              <c:f>fuselage!$R$3:$R$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -2106,7 +2163,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$S$3:$S$23</c:f>
+              <c:f>fuselage!$S$3:$S$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -2223,7 +2280,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$U$3:$U$23</c:f>
+              <c:f>fuselage!$U$3:$U$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -2295,7 +2352,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$V$3:$V$23</c:f>
+              <c:f>fuselage!$V$3:$V$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -2412,7 +2469,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$X$3:$X$23</c:f>
+              <c:f>fuselage!$X$3:$X$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -2484,7 +2541,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Y$3:$Y$23</c:f>
+              <c:f>fuselage!$Y$3:$Y$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -2630,7 +2687,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:rPr lang="en-US" sz="1600" b="1"/>
                   <a:t>Nominal Gross Weight (lb)</a:t>
                 </a:r>
               </a:p>
@@ -2764,22 +2821,22 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:rPr lang="en-US" sz="1600" b="1"/>
                   <a:t>Equivalent</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                  <a:rPr lang="en-US" sz="1600" b="1" baseline="0"/>
                   <a:t> Parasite Drag Area (ft</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1600" baseline="30000"/>
+                  <a:rPr lang="en-US" sz="1600" b="1" baseline="30000"/>
                   <a:t>2</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                  <a:rPr lang="en-US" sz="1600" b="1" baseline="0"/>
                   <a:t>)</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US" sz="1600"/>
+                <a:endParaRPr lang="en-US" sz="1600" b="1"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2991,6 +3048,1257 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12441044805947479"/>
+          <c:y val="2.3166545671152807E-2"/>
+          <c:w val="0.81244149168853896"/>
+          <c:h val="0.83398895450568666"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>K1.2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:prstDash val="dash"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>hub!$G$3:$G$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12250</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>26875</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31750</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>36625</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>46375</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>51250</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>56125</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>61000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>65875</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>70750</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>75625</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80500</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>85375</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>90250</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>95125</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>hub!$H$3:$H$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>2.2104188991842317</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.546626328200615</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.3768368409388918</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.9726304284355392</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.4217092926476287</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.766640893436543</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.032163714268366</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13.234260175439607</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14.384010028851337</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15.489492705389354</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16.556828840372123</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17.59079559175284</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18.595212087085613</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19.573192387510147</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>20.527317933009261</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>21.459758873047885</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>22.372361745881438</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>23.266714308031634</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>24.144194430252892</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>25.006007622889708</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>25.853216280382611</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-3A2B-184D-9A96-CF011E625D31}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>K0.85</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd" cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>hub!$J$3:$J$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11900</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21800</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31700</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>51500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>61400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>71300</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>81200</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>91100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>101000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>110900</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>120800</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>130700</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>140600</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150500</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>160400</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>170300</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>180200</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>190100</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>200000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>hub!$K$3:$K$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1.3492908941729693</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.43047441870059</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.633202485291009</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.5138324775029517</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.205034551656585</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.765861858241498</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.229126617005937</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14.615441723895216</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.93882412702223</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17.209351707886039</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18.434576922409022</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>19.620344254282262</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20.771293795591507</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>21.891187332393717</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>22.983128196861092</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>24.049714530031874</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>25.093149170225455</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>26.115320356229613</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>27.117862238512657</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>28.102201079362764</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>29.069591093503838</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3A2B-184D-9A96-CF011E625D31}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>K0.4</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>hub!$M$3:$M$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23800</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43600</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>63400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>83200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>103000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>122800</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>142600</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>162400</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>182200</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>202000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>221800</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>241600</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>261400</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>281200</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>301000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>320800</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>340600</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>360400</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>380200</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>400000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>hub!$N$3:$N$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1.0079368399158983</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.3096187072769476</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.9550835779148343</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.3599372381502155</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.6232859212571658</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.7892430546282707</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.8823197686850506</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.917914149407615</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11.906497028880565</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12.855596708136019</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13.770854964339193</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14.656637698459239</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15.516411116170586</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>16.352985317776341</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>17.168678530455193</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17.965431597415286</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>18.744890065887461</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>19.508464473395502</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>20.257375550373517</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20.992688732236388</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21.715340932759247</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000E-3A2B-184D-9A96-CF011E625D31}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Without fairing</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>hub!$D$5:$D$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>2695.2519510142101</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2580.3102304748199</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2972.93983249133</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4167.4828090921501</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4497.7658785029798</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4497.7658785029798</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5413.0057173572404</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2784.8060429336201</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7343.9650158852</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7505.7539204129998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7587.9800950090703</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7840.1029685888097</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7840.1029685888097</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10521.605614327</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9963.7474945948306</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12122.612259240301</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12941.582395224001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>13371.587337421901</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>12941.582395224001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>16627.240910203102</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>16092.5403106346</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>17367.912964078601</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23055.578575730498</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>18949.7080627377</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>22558.6082726038</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>21362.545308830198</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>30274.191602250699</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>41978.642582492401</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>45801.877488303398</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>41978.642582492401</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>46810.901301477803</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>46303.640964046703</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>62140.593137999102</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>hub!$C$5:$C$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>5.29101148916111</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.4116066740562201</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.39412553890896</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.74902389616391</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.9564741877088201</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.15653137601302</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.6896752211752202</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.70077831257333</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.2497379437393001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.0423607751005202</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.5413815755014202</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.0283071801380101</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.5270838162584504</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.1109354170654102</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.9839690488678698</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.53380060500265</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.39398145593064</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.1867619856537406</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.8045616937983695</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.44724533003233</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.6490409575756901</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.4864387144298199</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6.4394201383862004</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8.7407396225885297</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8.6773801816509408</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9.9636903277546605</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>15.083947351828099</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>11.951135288991299</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>14.7583000229055</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>15.756957145976999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>16.823190890198099</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>18.899977859593498</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>17.1944007970875</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-3A2B-184D-9A96-CF011E625D31}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>With fairing</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>hub!$D$3:$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>22314.1548028738</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4497.7658785029798</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>hub!$C$3:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>4.0130587103054003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8559334586276</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-3A2B-184D-9A96-CF011E625D31}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="378918464"/>
+        <c:axId val="378920176"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="378918464"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="1000000"/>
+          <c:min val="1000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" b="1"/>
+                  <a:t>Nominal Gross Weight (lb)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="378920176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="378920176"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" b="1"/>
+                  <a:t>Equivalent</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" b="1" baseline="0"/>
+                  <a:t> Parasite Drag Area (ft</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" b="1" baseline="30000"/>
+                  <a:t>2</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" b="1" baseline="0"/>
+                  <a:t>)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1600" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="378918464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3031,7 +4339,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3640,15 +5504,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>340180</xdr:colOff>
+      <xdr:colOff>365580</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>151214</xdr:rowOff>
+      <xdr:rowOff>163914</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>38219</xdr:colOff>
+      <xdr:colOff>63619</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>175148</xdr:rowOff>
+      <xdr:rowOff>187848</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -3663,7 +5527,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="8404680" y="5485214"/>
+          <a:off x="8430080" y="5497914"/>
           <a:ext cx="7127539" cy="5510334"/>
           <a:chOff x="7439480" y="5624914"/>
           <a:chExt cx="7127539" cy="5510334"/>
@@ -3690,8 +5554,8 @@
           </a:graphicData>
         </a:graphic>
       </xdr:graphicFrame>
-      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-        <mc:Choice Requires="a14">
+      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+        <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
               <xdr:cNvPr id="8" name="TextBox 7">
@@ -3883,7 +5747,7 @@
             </xdr:txBody>
           </xdr:sp>
         </mc:Choice>
-        <mc:Fallback xmlns="">
+        <mc:Fallback>
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
               <xdr:cNvPr id="8" name="TextBox 7">
@@ -4044,8 +5908,8 @@
           </a:fontRef>
         </xdr:style>
       </xdr:cxnSp>
-      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-        <mc:Choice Requires="a14">
+      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+        <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
               <xdr:cNvPr id="27" name="TextBox 26">
@@ -4242,7 +6106,7 @@
             </xdr:txBody>
           </xdr:sp>
         </mc:Choice>
-        <mc:Fallback xmlns="">
+        <mc:Fallback>
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
               <xdr:cNvPr id="27" name="TextBox 26">
@@ -4326,8 +6190,8 @@
           </xdr:sp>
         </mc:Fallback>
       </mc:AlternateContent>
-      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-        <mc:Choice Requires="a14">
+      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+        <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
               <xdr:cNvPr id="30" name="TextBox 29">
@@ -4524,7 +6388,7 @@
             </xdr:txBody>
           </xdr:sp>
         </mc:Choice>
-        <mc:Fallback xmlns="">
+        <mc:Fallback>
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
               <xdr:cNvPr id="30" name="TextBox 29">
@@ -4608,8 +6472,8 @@
           </xdr:sp>
         </mc:Fallback>
       </mc:AlternateContent>
-      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-        <mc:Choice Requires="a14">
+      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+        <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
               <xdr:cNvPr id="42" name="TextBox 41">
@@ -4794,7 +6658,7 @@
             </xdr:txBody>
           </xdr:sp>
         </mc:Choice>
-        <mc:Fallback xmlns="">
+        <mc:Fallback>
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
               <xdr:cNvPr id="42" name="TextBox 41">
@@ -4906,8 +6770,8 @@
           </a:fontRef>
         </xdr:style>
       </xdr:cxnSp>
-      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-        <mc:Choice Requires="a14">
+      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+        <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
               <xdr:cNvPr id="46" name="TextBox 45">
@@ -5112,7 +6976,7 @@
             </xdr:txBody>
           </xdr:sp>
         </mc:Choice>
-        <mc:Fallback xmlns="">
+        <mc:Fallback>
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
               <xdr:cNvPr id="46" name="TextBox 45">
@@ -5261,6 +7125,1226 @@
           <a:xfrm flipH="1" flipV="1">
             <a:off x="10826750" y="8001000"/>
             <a:ext cx="815910" cy="873969"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="3175">
+            <a:tailEnd type="none"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>369055</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>52919</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AEA68A4-8D7D-FE60-7E9C-259FB9997825}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11760200" y="572255"/>
+          <a:ext cx="5308600" cy="4598764"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>469901</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>203201</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="11" name="Group 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6C82293-6B32-EC42-74ED-C0E26532B249}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="6007101" y="5689600"/>
+          <a:ext cx="5486400" cy="5486400"/>
+          <a:chOff x="6007101" y="5689600"/>
+          <a:chExt cx="5486400" cy="5486400"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="28" name="Group 27">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FF26BEF-8228-C446-8104-621FF257FB83}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="6007101" y="5689600"/>
+            <a:ext cx="5486400" cy="5486400"/>
+            <a:chOff x="7439481" y="5624914"/>
+            <a:chExt cx="6915410" cy="5321300"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="29" name="Chart 28">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6453AA6B-C42F-E130-C23E-A465C39A6511}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="7439481" y="5624914"/>
+            <a:ext cx="6915410" cy="5321300"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+              <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+          <mc:Choice Requires="a14">
+            <xdr:sp macro="" textlink="">
+              <xdr:nvSpPr>
+                <xdr:cNvPr id="30" name="TextBox 29">
+                  <a:extLst>
+                    <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADBB1924-8AD2-5A59-8C5F-D690EF44CBDB}"/>
+                    </a:ext>
+                  </a:extLst>
+                </xdr:cNvPr>
+                <xdr:cNvSpPr txBox="1"/>
+              </xdr:nvSpPr>
+              <xdr:spPr>
+                <a:xfrm>
+                  <a:off x="11289867" y="8857976"/>
+                  <a:ext cx="2488738" cy="819502"/>
+                </a:xfrm>
+                <a:prstGeom prst="rect">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:ln w="9525" cmpd="sng">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:shade val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+              </xdr:spPr>
+              <xdr:style>
+                <a:lnRef idx="0">
+                  <a:scrgbClr r="0" g="0" b="0"/>
+                </a:lnRef>
+                <a:fillRef idx="0">
+                  <a:scrgbClr r="0" g="0" b="0"/>
+                </a:fillRef>
+                <a:effectRef idx="0">
+                  <a:scrgbClr r="0" g="0" b="0"/>
+                </a:effectRef>
+                <a:fontRef idx="minor">
+                  <a:schemeClr val="dk1"/>
+                </a:fontRef>
+              </xdr:style>
+              <xdr:txBody>
+                <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr algn="ctr"/>
+                  <a:r>
+                    <a:rPr lang="en-US" sz="1300" i="0"/>
+                    <a:t>Present</a:t>
+                  </a:r>
+                  <a:r>
+                    <a:rPr lang="en-US" sz="1300" i="0" baseline="0"/>
+                    <a:t> heavy lift</a:t>
+                  </a:r>
+                </a:p>
+                <a:p>
+                  <a:pPr algn="ctr"/>
+                  <a:r>
+                    <a:rPr lang="en-US" sz="1300" i="0" baseline="0"/>
+                    <a:t>compound helicopter</a:t>
+                  </a:r>
+                  <a:r>
+                    <a:rPr lang="en-US" sz="1300" i="0"/>
+                    <a:t> </a:t>
+                  </a:r>
+                </a:p>
+                <a:p>
+                  <a:pPr algn="ctr"/>
+                  <a14:m>
+                    <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                      <m:sSub>
+                        <m:sSubPr>
+                          <m:ctrlPr>
+                            <a:rPr lang="en-US" sz="1300" b="0" i="1">
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            </a:rPr>
+                          </m:ctrlPr>
+                        </m:sSubPr>
+                        <m:e>
+                          <m:r>
+                            <m:rPr>
+                              <m:sty m:val="p"/>
+                            </m:rPr>
+                            <a:rPr lang="en-US" sz="1300" b="0" i="0">
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            </a:rPr>
+                            <m:t>f</m:t>
+                          </m:r>
+                        </m:e>
+                        <m:sub>
+                          <m:r>
+                            <m:rPr>
+                              <m:sty m:val="p"/>
+                            </m:rPr>
+                            <a:rPr lang="en-US" sz="1300" b="0" i="0">
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            </a:rPr>
+                            <m:t>e</m:t>
+                          </m:r>
+                        </m:sub>
+                      </m:sSub>
+                      <m:r>
+                        <a:rPr lang="en-US" sz="1300" b="0" i="0">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>=0.40 </m:t>
+                      </m:r>
+                      <m:sSup>
+                        <m:sSupPr>
+                          <m:ctrlPr>
+                            <a:rPr lang="en-US" sz="1300" b="0" i="1">
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            </a:rPr>
+                          </m:ctrlPr>
+                        </m:sSupPr>
+                        <m:e>
+                          <m:d>
+                            <m:dPr>
+                              <m:ctrlPr>
+                                <a:rPr lang="en-US" sz="1300" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                              </m:ctrlPr>
+                            </m:dPr>
+                            <m:e>
+                              <m:f>
+                                <m:fPr>
+                                  <m:type m:val="lin"/>
+                                  <m:ctrlPr>
+                                    <a:rPr lang="en-US" sz="1300" b="0" i="1">
+                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    </a:rPr>
+                                  </m:ctrlPr>
+                                </m:fPr>
+                                <m:num>
+                                  <m:r>
+                                    <m:rPr>
+                                      <m:sty m:val="p"/>
+                                    </m:rPr>
+                                    <a:rPr lang="en-US" sz="1300" b="0" i="0">
+                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    </a:rPr>
+                                    <m:t>GW</m:t>
+                                  </m:r>
+                                </m:num>
+                                <m:den>
+                                  <m:r>
+                                    <a:rPr lang="en-US" sz="1300" b="0" i="1">
+                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    </a:rPr>
+                                    <m:t>1000</m:t>
+                                  </m:r>
+                                </m:den>
+                              </m:f>
+                            </m:e>
+                          </m:d>
+                        </m:e>
+                        <m:sup>
+                          <m:f>
+                            <m:fPr>
+                              <m:type m:val="lin"/>
+                              <m:ctrlPr>
+                                <a:rPr lang="en-US" sz="1300" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                              </m:ctrlPr>
+                            </m:fPr>
+                            <m:num>
+                              <m:r>
+                                <a:rPr lang="en-US" sz="1300" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>2</m:t>
+                              </m:r>
+                            </m:num>
+                            <m:den>
+                              <m:r>
+                                <a:rPr lang="en-US" sz="1300" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>3</m:t>
+                              </m:r>
+                            </m:den>
+                          </m:f>
+                        </m:sup>
+                      </m:sSup>
+                    </m:oMath>
+                  </a14:m>
+                  <a:r>
+                    <a:rPr lang="en-US" sz="1300" i="0"/>
+                    <a:t> </a:t>
+                  </a:r>
+                </a:p>
+              </xdr:txBody>
+            </xdr:sp>
+          </mc:Choice>
+          <mc:Fallback xmlns="">
+            <xdr:sp macro="" textlink="">
+              <xdr:nvSpPr>
+                <xdr:cNvPr id="30" name="TextBox 29">
+                  <a:extLst>
+                    <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADBB1924-8AD2-5A59-8C5F-D690EF44CBDB}"/>
+                    </a:ext>
+                  </a:extLst>
+                </xdr:cNvPr>
+                <xdr:cNvSpPr txBox="1"/>
+              </xdr:nvSpPr>
+              <xdr:spPr>
+                <a:xfrm>
+                  <a:off x="11289867" y="8857976"/>
+                  <a:ext cx="2488738" cy="819502"/>
+                </a:xfrm>
+                <a:prstGeom prst="rect">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:ln w="9525" cmpd="sng">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:shade val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+              </xdr:spPr>
+              <xdr:style>
+                <a:lnRef idx="0">
+                  <a:scrgbClr r="0" g="0" b="0"/>
+                </a:lnRef>
+                <a:fillRef idx="0">
+                  <a:scrgbClr r="0" g="0" b="0"/>
+                </a:fillRef>
+                <a:effectRef idx="0">
+                  <a:scrgbClr r="0" g="0" b="0"/>
+                </a:effectRef>
+                <a:fontRef idx="minor">
+                  <a:schemeClr val="dk1"/>
+                </a:fontRef>
+              </xdr:style>
+              <xdr:txBody>
+                <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr algn="ctr"/>
+                  <a:r>
+                    <a:rPr lang="en-US" sz="1300" i="0"/>
+                    <a:t>Present</a:t>
+                  </a:r>
+                  <a:r>
+                    <a:rPr lang="en-US" sz="1300" i="0" baseline="0"/>
+                    <a:t> heavy lift</a:t>
+                  </a:r>
+                </a:p>
+                <a:p>
+                  <a:pPr algn="ctr"/>
+                  <a:r>
+                    <a:rPr lang="en-US" sz="1300" i="0" baseline="0"/>
+                    <a:t>compound helicopter</a:t>
+                  </a:r>
+                  <a:r>
+                    <a:rPr lang="en-US" sz="1300" i="0"/>
+                    <a:t> </a:t>
+                  </a:r>
+                </a:p>
+                <a:p>
+                  <a:pPr algn="ctr"/>
+                  <a:r>
+                    <a:rPr lang="en-US" sz="1300" b="0" i="0">
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    </a:rPr>
+                    <a:t>f_e=0.40 (GW∕1000)^(2∕3)</a:t>
+                  </a:r>
+                  <a:r>
+                    <a:rPr lang="en-US" sz="1300" i="0"/>
+                    <a:t> </a:t>
+                  </a:r>
+                </a:p>
+              </xdr:txBody>
+            </xdr:sp>
+          </mc:Fallback>
+        </mc:AlternateContent>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="31" name="Straight Arrow Connector 30">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9CAF1E1-D8A0-2218-26E9-2C41D2B99DB8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr>
+              <a:cxnSpLocks/>
+              <a:stCxn id="34" idx="2"/>
+            </xdr:cNvCxnSpPr>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9835687" y="7312456"/>
+              <a:ext cx="1125529" cy="517349"/>
+            </a:xfrm>
+            <a:prstGeom prst="straightConnector1">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln w="3175">
+              <a:tailEnd type="none"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="dk1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="dk1"/>
+            </a:fillRef>
+            <a:effectRef idx="1">
+              <a:schemeClr val="dk1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="32" name="Straight Arrow Connector 31">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E59E93E2-5B2D-71DC-62DC-4036A3CA537B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr>
+              <a:cxnSpLocks/>
+              <a:stCxn id="33" idx="0"/>
+            </xdr:cNvCxnSpPr>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm flipH="1" flipV="1">
+              <a:off x="9581704" y="9642700"/>
+              <a:ext cx="1224322" cy="190730"/>
+            </a:xfrm>
+            <a:prstGeom prst="straightConnector1">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln w="3175">
+              <a:tailEnd type="none"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="dk1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="dk1"/>
+            </a:fillRef>
+            <a:effectRef idx="1">
+              <a:schemeClr val="dk1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="33" name="TextBox 32">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2ECD3E1-B5A3-00C8-3A4F-895A91285E43}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="10138581" y="9833431"/>
+              <a:ext cx="1334888" cy="262854"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1300" i="0"/>
+                <a:t>Faired</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1300" i="0" baseline="0"/>
+                <a:t> Hubs</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1300" i="0"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+          <mc:Choice Requires="a14">
+            <xdr:sp macro="" textlink="">
+              <xdr:nvSpPr>
+                <xdr:cNvPr id="34" name="TextBox 33">
+                  <a:extLst>
+                    <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD625480-1BA9-54EA-6684-63954C806E53}"/>
+                    </a:ext>
+                  </a:extLst>
+                </xdr:cNvPr>
+                <xdr:cNvSpPr txBox="1"/>
+              </xdr:nvSpPr>
+              <xdr:spPr>
+                <a:xfrm>
+                  <a:off x="8614110" y="6778361"/>
+                  <a:ext cx="2443154" cy="534095"/>
+                </a:xfrm>
+                <a:prstGeom prst="rect">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:ln w="9525" cmpd="sng">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:shade val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+              </xdr:spPr>
+              <xdr:style>
+                <a:lnRef idx="0">
+                  <a:scrgbClr r="0" g="0" b="0"/>
+                </a:lnRef>
+                <a:fillRef idx="0">
+                  <a:scrgbClr r="0" g="0" b="0"/>
+                </a:fillRef>
+                <a:effectRef idx="0">
+                  <a:scrgbClr r="0" g="0" b="0"/>
+                </a:effectRef>
+                <a:fontRef idx="minor">
+                  <a:schemeClr val="dk1"/>
+                </a:fontRef>
+              </xdr:style>
+              <xdr:txBody>
+                <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr algn="ctr"/>
+                  <a:r>
+                    <a:rPr lang="en-US" sz="1300" i="0"/>
+                    <a:t>Typical</a:t>
+                  </a:r>
+                  <a:r>
+                    <a:rPr lang="en-US" sz="1300" i="0" baseline="0"/>
+                    <a:t> Hub Technology</a:t>
+                  </a:r>
+                  <a:endParaRPr lang="en-US" sz="1300" i="0"/>
+                </a:p>
+                <a:p>
+                  <a:pPr algn="ctr"/>
+                  <a14:m>
+                    <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                      <m:sSub>
+                        <m:sSubPr>
+                          <m:ctrlPr>
+                            <a:rPr lang="en-US" sz="1300" b="0" i="1">
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            </a:rPr>
+                          </m:ctrlPr>
+                        </m:sSubPr>
+                        <m:e>
+                          <m:r>
+                            <m:rPr>
+                              <m:sty m:val="p"/>
+                            </m:rPr>
+                            <a:rPr lang="en-US" sz="1300" b="0" i="0">
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            </a:rPr>
+                            <m:t>f</m:t>
+                          </m:r>
+                        </m:e>
+                        <m:sub>
+                          <m:r>
+                            <m:rPr>
+                              <m:sty m:val="p"/>
+                            </m:rPr>
+                            <a:rPr lang="en-US" sz="1300" b="0" i="0">
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            </a:rPr>
+                            <m:t>e</m:t>
+                          </m:r>
+                        </m:sub>
+                      </m:sSub>
+                      <m:r>
+                        <a:rPr lang="en-US" sz="1300" b="0" i="0">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>=1.20 </m:t>
+                      </m:r>
+                      <m:sSup>
+                        <m:sSupPr>
+                          <m:ctrlPr>
+                            <a:rPr lang="en-US" sz="1300" b="0" i="1">
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            </a:rPr>
+                          </m:ctrlPr>
+                        </m:sSupPr>
+                        <m:e>
+                          <m:d>
+                            <m:dPr>
+                              <m:ctrlPr>
+                                <a:rPr lang="en-US" sz="1300" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                              </m:ctrlPr>
+                            </m:dPr>
+                            <m:e>
+                              <m:f>
+                                <m:fPr>
+                                  <m:type m:val="lin"/>
+                                  <m:ctrlPr>
+                                    <a:rPr lang="en-US" sz="1300" b="0" i="1">
+                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    </a:rPr>
+                                  </m:ctrlPr>
+                                </m:fPr>
+                                <m:num>
+                                  <m:r>
+                                    <m:rPr>
+                                      <m:sty m:val="p"/>
+                                    </m:rPr>
+                                    <a:rPr lang="en-US" sz="1300" b="0" i="0">
+                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    </a:rPr>
+                                    <m:t>GW</m:t>
+                                  </m:r>
+                                </m:num>
+                                <m:den>
+                                  <m:r>
+                                    <a:rPr lang="en-US" sz="1300" b="0" i="1">
+                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    </a:rPr>
+                                    <m:t>1000</m:t>
+                                  </m:r>
+                                </m:den>
+                              </m:f>
+                            </m:e>
+                          </m:d>
+                        </m:e>
+                        <m:sup>
+                          <m:f>
+                            <m:fPr>
+                              <m:type m:val="lin"/>
+                              <m:ctrlPr>
+                                <a:rPr lang="en-US" sz="1300" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                              </m:ctrlPr>
+                            </m:fPr>
+                            <m:num>
+                              <m:r>
+                                <a:rPr lang="en-US" sz="1300" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>2</m:t>
+                              </m:r>
+                            </m:num>
+                            <m:den>
+                              <m:r>
+                                <a:rPr lang="en-US" sz="1300" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>3</m:t>
+                              </m:r>
+                            </m:den>
+                          </m:f>
+                        </m:sup>
+                      </m:sSup>
+                    </m:oMath>
+                  </a14:m>
+                  <a:r>
+                    <a:rPr lang="en-US" sz="1300" i="0"/>
+                    <a:t> </a:t>
+                  </a:r>
+                </a:p>
+              </xdr:txBody>
+            </xdr:sp>
+          </mc:Choice>
+          <mc:Fallback xmlns="">
+            <xdr:sp macro="" textlink="">
+              <xdr:nvSpPr>
+                <xdr:cNvPr id="34" name="TextBox 33">
+                  <a:extLst>
+                    <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD625480-1BA9-54EA-6684-63954C806E53}"/>
+                    </a:ext>
+                  </a:extLst>
+                </xdr:cNvPr>
+                <xdr:cNvSpPr txBox="1"/>
+              </xdr:nvSpPr>
+              <xdr:spPr>
+                <a:xfrm>
+                  <a:off x="8614110" y="6778361"/>
+                  <a:ext cx="2443154" cy="534095"/>
+                </a:xfrm>
+                <a:prstGeom prst="rect">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:ln w="9525" cmpd="sng">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:shade val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+              </xdr:spPr>
+              <xdr:style>
+                <a:lnRef idx="0">
+                  <a:scrgbClr r="0" g="0" b="0"/>
+                </a:lnRef>
+                <a:fillRef idx="0">
+                  <a:scrgbClr r="0" g="0" b="0"/>
+                </a:fillRef>
+                <a:effectRef idx="0">
+                  <a:scrgbClr r="0" g="0" b="0"/>
+                </a:effectRef>
+                <a:fontRef idx="minor">
+                  <a:schemeClr val="dk1"/>
+                </a:fontRef>
+              </xdr:style>
+              <xdr:txBody>
+                <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr algn="ctr"/>
+                  <a:r>
+                    <a:rPr lang="en-US" sz="1300" i="0"/>
+                    <a:t>Typical</a:t>
+                  </a:r>
+                  <a:r>
+                    <a:rPr lang="en-US" sz="1300" i="0" baseline="0"/>
+                    <a:t> Hub Technology</a:t>
+                  </a:r>
+                  <a:endParaRPr lang="en-US" sz="1300" i="0"/>
+                </a:p>
+                <a:p>
+                  <a:pPr algn="ctr"/>
+                  <a:r>
+                    <a:rPr lang="en-US" sz="1300" b="0" i="0">
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    </a:rPr>
+                    <a:t>f_e=1.20 (GW∕1000)^(2∕3)</a:t>
+                  </a:r>
+                  <a:r>
+                    <a:rPr lang="en-US" sz="1300" i="0"/>
+                    <a:t> </a:t>
+                  </a:r>
+                </a:p>
+              </xdr:txBody>
+            </xdr:sp>
+          </mc:Fallback>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+          <mc:Choice Requires="a14">
+            <xdr:sp macro="" textlink="">
+              <xdr:nvSpPr>
+                <xdr:cNvPr id="37" name="TextBox 36">
+                  <a:extLst>
+                    <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2880D47B-17DC-4D30-E40A-F68302638676}"/>
+                    </a:ext>
+                  </a:extLst>
+                </xdr:cNvPr>
+                <xdr:cNvSpPr txBox="1"/>
+              </xdr:nvSpPr>
+              <xdr:spPr>
+                <a:xfrm>
+                  <a:off x="11150963" y="5943179"/>
+                  <a:ext cx="2515588" cy="556300"/>
+                </a:xfrm>
+                <a:prstGeom prst="rect">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:ln w="9525" cmpd="sng">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:shade val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+              </xdr:spPr>
+              <xdr:style>
+                <a:lnRef idx="0">
+                  <a:scrgbClr r="0" g="0" b="0"/>
+                </a:lnRef>
+                <a:fillRef idx="0">
+                  <a:scrgbClr r="0" g="0" b="0"/>
+                </a:fillRef>
+                <a:effectRef idx="0">
+                  <a:scrgbClr r="0" g="0" b="0"/>
+                </a:effectRef>
+                <a:fontRef idx="minor">
+                  <a:schemeClr val="dk1"/>
+                </a:fontRef>
+              </xdr:style>
+              <xdr:txBody>
+                <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr algn="ctr"/>
+                  <a:r>
+                    <a:rPr lang="en-US" sz="1300" i="0"/>
+                    <a:t>Possible</a:t>
+                  </a:r>
+                  <a:r>
+                    <a:rPr lang="en-US" sz="1300" i="0" baseline="0"/>
+                    <a:t> Hub Technology</a:t>
+                  </a:r>
+                  <a:endParaRPr lang="en-US" sz="1300" i="0"/>
+                </a:p>
+                <a:p>
+                  <a:pPr algn="ctr"/>
+                  <a14:m>
+                    <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                      <m:sSub>
+                        <m:sSubPr>
+                          <m:ctrlPr>
+                            <a:rPr lang="en-US" sz="1300" b="0" i="1">
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            </a:rPr>
+                          </m:ctrlPr>
+                        </m:sSubPr>
+                        <m:e>
+                          <m:r>
+                            <m:rPr>
+                              <m:sty m:val="p"/>
+                            </m:rPr>
+                            <a:rPr lang="en-US" sz="1300" b="0" i="0">
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            </a:rPr>
+                            <m:t>f</m:t>
+                          </m:r>
+                        </m:e>
+                        <m:sub>
+                          <m:r>
+                            <m:rPr>
+                              <m:sty m:val="p"/>
+                            </m:rPr>
+                            <a:rPr lang="en-US" sz="1300" b="0" i="0">
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            </a:rPr>
+                            <m:t>e</m:t>
+                          </m:r>
+                        </m:sub>
+                      </m:sSub>
+                      <m:r>
+                        <a:rPr lang="en-US" sz="1300" b="0" i="0">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>=0.85 </m:t>
+                      </m:r>
+                      <m:sSup>
+                        <m:sSupPr>
+                          <m:ctrlPr>
+                            <a:rPr lang="en-US" sz="1300" b="0" i="1">
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            </a:rPr>
+                          </m:ctrlPr>
+                        </m:sSupPr>
+                        <m:e>
+                          <m:d>
+                            <m:dPr>
+                              <m:ctrlPr>
+                                <a:rPr lang="en-US" sz="1300" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                              </m:ctrlPr>
+                            </m:dPr>
+                            <m:e>
+                              <m:f>
+                                <m:fPr>
+                                  <m:type m:val="lin"/>
+                                  <m:ctrlPr>
+                                    <a:rPr lang="en-US" sz="1300" b="0" i="1">
+                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    </a:rPr>
+                                  </m:ctrlPr>
+                                </m:fPr>
+                                <m:num>
+                                  <m:r>
+                                    <m:rPr>
+                                      <m:sty m:val="p"/>
+                                    </m:rPr>
+                                    <a:rPr lang="en-US" sz="1300" b="0" i="0">
+                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    </a:rPr>
+                                    <m:t>GW</m:t>
+                                  </m:r>
+                                </m:num>
+                                <m:den>
+                                  <m:r>
+                                    <a:rPr lang="en-US" sz="1300" b="0" i="1">
+                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    </a:rPr>
+                                    <m:t>1000</m:t>
+                                  </m:r>
+                                </m:den>
+                              </m:f>
+                            </m:e>
+                          </m:d>
+                        </m:e>
+                        <m:sup>
+                          <m:f>
+                            <m:fPr>
+                              <m:type m:val="lin"/>
+                              <m:ctrlPr>
+                                <a:rPr lang="en-US" sz="1300" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                              </m:ctrlPr>
+                            </m:fPr>
+                            <m:num>
+                              <m:r>
+                                <a:rPr lang="en-US" sz="1300" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>2</m:t>
+                              </m:r>
+                            </m:num>
+                            <m:den>
+                              <m:r>
+                                <a:rPr lang="en-US" sz="1300" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>3</m:t>
+                              </m:r>
+                            </m:den>
+                          </m:f>
+                        </m:sup>
+                      </m:sSup>
+                    </m:oMath>
+                  </a14:m>
+                  <a:r>
+                    <a:rPr lang="en-US" sz="1300" i="0"/>
+                    <a:t> </a:t>
+                  </a:r>
+                </a:p>
+              </xdr:txBody>
+            </xdr:sp>
+          </mc:Choice>
+          <mc:Fallback xmlns="">
+            <xdr:sp macro="" textlink="">
+              <xdr:nvSpPr>
+                <xdr:cNvPr id="37" name="TextBox 36">
+                  <a:extLst>
+                    <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2880D47B-17DC-4D30-E40A-F68302638676}"/>
+                    </a:ext>
+                  </a:extLst>
+                </xdr:cNvPr>
+                <xdr:cNvSpPr txBox="1"/>
+              </xdr:nvSpPr>
+              <xdr:spPr>
+                <a:xfrm>
+                  <a:off x="11150963" y="5943179"/>
+                  <a:ext cx="2515588" cy="556300"/>
+                </a:xfrm>
+                <a:prstGeom prst="rect">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:ln w="9525" cmpd="sng">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:shade val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+              </xdr:spPr>
+              <xdr:style>
+                <a:lnRef idx="0">
+                  <a:scrgbClr r="0" g="0" b="0"/>
+                </a:lnRef>
+                <a:fillRef idx="0">
+                  <a:scrgbClr r="0" g="0" b="0"/>
+                </a:fillRef>
+                <a:effectRef idx="0">
+                  <a:scrgbClr r="0" g="0" b="0"/>
+                </a:effectRef>
+                <a:fontRef idx="minor">
+                  <a:schemeClr val="dk1"/>
+                </a:fontRef>
+              </xdr:style>
+              <xdr:txBody>
+                <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr algn="ctr"/>
+                  <a:r>
+                    <a:rPr lang="en-US" sz="1300" i="0"/>
+                    <a:t>Possible</a:t>
+                  </a:r>
+                  <a:r>
+                    <a:rPr lang="en-US" sz="1300" i="0" baseline="0"/>
+                    <a:t> Hub Technology</a:t>
+                  </a:r>
+                  <a:endParaRPr lang="en-US" sz="1300" i="0"/>
+                </a:p>
+                <a:p>
+                  <a:pPr algn="ctr"/>
+                  <a:r>
+                    <a:rPr lang="en-US" sz="1300" b="0" i="0">
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    </a:rPr>
+                    <a:t>f_e=0.85 (GW∕1000)^(2∕3)</a:t>
+                  </a:r>
+                  <a:r>
+                    <a:rPr lang="en-US" sz="1300" i="0"/>
+                    <a:t> </a:t>
+                  </a:r>
+                </a:p>
+              </xdr:txBody>
+            </xdr:sp>
+          </mc:Fallback>
+        </mc:AlternateContent>
+      </xdr:grpSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="48" name="Straight Arrow Connector 47">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{949AADFC-FB9C-4445-8CBA-657550AF3E40}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:cxnSpLocks/>
+            <a:stCxn id="33" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="8677978" y="9067800"/>
+            <a:ext cx="21522" cy="960892"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="3175">
+            <a:tailEnd type="none"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="58" name="Straight Arrow Connector 57">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6E51F9D-D5AE-7643-A6FB-6599E3A6C1CB}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:cxnSpLocks/>
+            <a:endCxn id="37" idx="2"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1" flipV="1">
+            <a:off x="9949519" y="6591300"/>
+            <a:ext cx="7281" cy="546100"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="3175">
+            <a:tailEnd type="none"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="64" name="Straight Arrow Connector 63">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{871F2B27-25F8-CA48-BED1-5039CA9652E7}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="30" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1" flipV="1">
+            <a:off x="9613900" y="8382000"/>
+            <a:ext cx="435169" cy="640972"/>
           </a:xfrm>
           <a:prstGeom prst="straightConnector1">
             <a:avLst/>
@@ -5609,8 +8693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{794DF518-2B61-2646-92A6-1D07C212A41D}">
   <dimension ref="B2:Y102"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScaleNormal="159" workbookViewId="0">
-      <selection activeCell="R43" sqref="R43"/>
+    <sheetView tabSelected="1" topLeftCell="E17" zoomScaleNormal="159" workbookViewId="0">
+      <selection activeCell="T32" sqref="T32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8656,11 +11740,1173 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FCEE61-850F-6442-B4AC-A1CE2F893CD8}">
+  <dimension ref="B2:O73"/>
+  <sheetViews>
+    <sheetView topLeftCell="C16" workbookViewId="0">
+      <selection activeCell="R44" sqref="R44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="6.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="3.83203125" customWidth="1"/>
+    <col min="12" max="12" width="3.1640625" customWidth="1"/>
+    <col min="15" max="15" width="3.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:15" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="N2" s="27">
+        <v>0.4</v>
+      </c>
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B3" s="9">
+        <v>1</v>
+      </c>
+      <c r="C3" s="34">
+        <v>4.0130587103054003</v>
+      </c>
+      <c r="D3" s="32">
+        <v>22314.1548028738</v>
+      </c>
+      <c r="E3" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" cm="1">
+        <f t="array" ref="G3:G23">_xlfn.SEQUENCE(21,1,2500,(100000-2500)/20)</f>
+        <v>2500</v>
+      </c>
+      <c r="H3" s="1">
+        <f>$H$2*(G3/1000)^(2/3)</f>
+        <v>2.2104188991842317</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1" cm="1">
+        <f t="array" ref="J3:J23">_xlfn.SEQUENCE(21,1,2000,(200000-2000)/20)</f>
+        <v>2000</v>
+      </c>
+      <c r="K3" s="1">
+        <f>$K$2*(J3/1000)^(2/3)</f>
+        <v>1.3492908941729693</v>
+      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1" cm="1">
+        <f t="array" ref="M3:M23">_xlfn.SEQUENCE(21,1,4000,(400000-4000)/20)</f>
+        <v>4000</v>
+      </c>
+      <c r="N3" s="1">
+        <f>$N$2*(M3/1000)^(2/3)</f>
+        <v>1.0079368399158983</v>
+      </c>
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B4" s="30">
+        <v>2</v>
+      </c>
+      <c r="C4" s="35">
+        <v>1.8559334586276</v>
+      </c>
+      <c r="D4" s="33">
+        <v>4497.7658785029798</v>
+      </c>
+      <c r="E4" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>7375</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" ref="H4:H23" si="0">$H$2*(G4/1000)^(2/3)</f>
+        <v>4.546626328200615</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1">
+        <v>11900</v>
+      </c>
+      <c r="K4" s="1">
+        <f t="shared" ref="K4:K23" si="1">$K$2*(J4/1000)^(2/3)</f>
+        <v>4.43047441870059</v>
+      </c>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1">
+        <v>23800</v>
+      </c>
+      <c r="N4" s="1">
+        <f t="shared" ref="N4:N23" si="2">$N$2*(M4/1000)^(2/3)</f>
+        <v>3.3096187072769476</v>
+      </c>
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B5" s="30">
+        <v>3</v>
+      </c>
+      <c r="C5" s="35">
+        <v>5.29101148916111</v>
+      </c>
+      <c r="D5" s="33">
+        <v>2695.2519510142101</v>
+      </c>
+      <c r="E5" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>12250</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="0"/>
+        <v>6.3768368409388918</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1">
+        <v>21800</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="shared" si="1"/>
+        <v>6.633202485291009</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1">
+        <v>43600</v>
+      </c>
+      <c r="N5" s="1">
+        <f t="shared" si="2"/>
+        <v>4.9550835779148343</v>
+      </c>
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B6" s="30">
+        <v>4</v>
+      </c>
+      <c r="C6" s="35">
+        <v>2.4116066740562201</v>
+      </c>
+      <c r="D6" s="33">
+        <v>2580.3102304748199</v>
+      </c>
+      <c r="E6" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>17125</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="0"/>
+        <v>7.9726304284355392</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1">
+        <v>31700</v>
+      </c>
+      <c r="K6" s="1">
+        <f t="shared" si="1"/>
+        <v>8.5138324775029517</v>
+      </c>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1">
+        <v>63400</v>
+      </c>
+      <c r="N6" s="1">
+        <f t="shared" si="2"/>
+        <v>6.3599372381502155</v>
+      </c>
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B7" s="30">
+        <v>5</v>
+      </c>
+      <c r="C7" s="35">
+        <v>2.39412553890896</v>
+      </c>
+      <c r="D7" s="33">
+        <v>2972.93983249133</v>
+      </c>
+      <c r="E7" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>22000</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="0"/>
+        <v>9.4217092926476287</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1">
+        <v>41600</v>
+      </c>
+      <c r="K7" s="1">
+        <f t="shared" si="1"/>
+        <v>10.205034551656585</v>
+      </c>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1">
+        <v>83200</v>
+      </c>
+      <c r="N7" s="1">
+        <f t="shared" si="2"/>
+        <v>7.6232859212571658</v>
+      </c>
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B8" s="30">
+        <v>6</v>
+      </c>
+      <c r="C8" s="35">
+        <v>2.74902389616391</v>
+      </c>
+      <c r="D8" s="33">
+        <v>4167.4828090921501</v>
+      </c>
+      <c r="E8" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>26875</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="0"/>
+        <v>10.766640893436543</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1">
+        <v>51500</v>
+      </c>
+      <c r="K8" s="1">
+        <f t="shared" si="1"/>
+        <v>11.765861858241498</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1">
+        <v>103000</v>
+      </c>
+      <c r="N8" s="1">
+        <f t="shared" si="2"/>
+        <v>8.7892430546282707</v>
+      </c>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B9" s="30">
+        <v>7</v>
+      </c>
+      <c r="C9" s="35">
+        <v>2.9564741877088201</v>
+      </c>
+      <c r="D9" s="33">
+        <v>4497.7658785029798</v>
+      </c>
+      <c r="E9" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>31750</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="0"/>
+        <v>12.032163714268366</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1">
+        <v>61400</v>
+      </c>
+      <c r="K9" s="1">
+        <f t="shared" si="1"/>
+        <v>13.229126617005937</v>
+      </c>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1">
+        <v>122800</v>
+      </c>
+      <c r="N9" s="1">
+        <f t="shared" si="2"/>
+        <v>9.8823197686850506</v>
+      </c>
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B10" s="30">
+        <v>8</v>
+      </c>
+      <c r="C10" s="35">
+        <v>3.15653137601302</v>
+      </c>
+      <c r="D10" s="33">
+        <v>4497.7658785029798</v>
+      </c>
+      <c r="E10" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>36625</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="0"/>
+        <v>13.234260175439607</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1">
+        <v>71300</v>
+      </c>
+      <c r="K10" s="1">
+        <f t="shared" si="1"/>
+        <v>14.615441723895216</v>
+      </c>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1">
+        <v>142600</v>
+      </c>
+      <c r="N10" s="1">
+        <f t="shared" si="2"/>
+        <v>10.917914149407615</v>
+      </c>
+      <c r="O10" s="1"/>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B11" s="30">
+        <v>9</v>
+      </c>
+      <c r="C11" s="35">
+        <v>2.6896752211752202</v>
+      </c>
+      <c r="D11" s="33">
+        <v>5413.0057173572404</v>
+      </c>
+      <c r="E11" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>41500</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="0"/>
+        <v>14.384010028851337</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1">
+        <v>81200</v>
+      </c>
+      <c r="K11" s="1">
+        <f t="shared" si="1"/>
+        <v>15.93882412702223</v>
+      </c>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1">
+        <v>162400</v>
+      </c>
+      <c r="N11" s="1">
+        <f t="shared" si="2"/>
+        <v>11.906497028880565</v>
+      </c>
+      <c r="O11" s="1"/>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B12" s="30">
+        <v>10</v>
+      </c>
+      <c r="C12" s="35">
+        <v>1.70077831257333</v>
+      </c>
+      <c r="D12" s="33">
+        <v>2784.8060429336201</v>
+      </c>
+      <c r="E12" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>46375</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="0"/>
+        <v>15.489492705389354</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1">
+        <v>91100</v>
+      </c>
+      <c r="K12" s="1">
+        <f t="shared" si="1"/>
+        <v>17.209351707886039</v>
+      </c>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1">
+        <v>182200</v>
+      </c>
+      <c r="N12" s="1">
+        <f t="shared" si="2"/>
+        <v>12.855596708136019</v>
+      </c>
+      <c r="O12" s="1"/>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B13" s="30">
+        <v>11</v>
+      </c>
+      <c r="C13" s="35">
+        <v>3.2497379437393001</v>
+      </c>
+      <c r="D13" s="33">
+        <v>7343.9650158852</v>
+      </c>
+      <c r="E13" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <v>51250</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="0"/>
+        <v>16.556828840372123</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1">
+        <v>101000</v>
+      </c>
+      <c r="K13" s="1">
+        <f t="shared" si="1"/>
+        <v>18.434576922409022</v>
+      </c>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1">
+        <v>202000</v>
+      </c>
+      <c r="N13" s="1">
+        <f t="shared" si="2"/>
+        <v>13.770854964339193</v>
+      </c>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B14" s="30">
+        <v>12</v>
+      </c>
+      <c r="C14" s="35">
+        <v>4.0423607751005202</v>
+      </c>
+      <c r="D14" s="33">
+        <v>7505.7539204129998</v>
+      </c>
+      <c r="E14" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <v>56125</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="0"/>
+        <v>17.59079559175284</v>
+      </c>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1">
+        <v>110900</v>
+      </c>
+      <c r="K14" s="1">
+        <f t="shared" si="1"/>
+        <v>19.620344254282262</v>
+      </c>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1">
+        <v>221800</v>
+      </c>
+      <c r="N14" s="1">
+        <f t="shared" si="2"/>
+        <v>14.656637698459239</v>
+      </c>
+      <c r="O14" s="1"/>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B15" s="30">
+        <v>13</v>
+      </c>
+      <c r="C15" s="35">
+        <v>4.5413815755014202</v>
+      </c>
+      <c r="D15" s="33">
+        <v>7587.9800950090703</v>
+      </c>
+      <c r="E15" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <v>61000</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" si="0"/>
+        <v>18.595212087085613</v>
+      </c>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1">
+        <v>120800</v>
+      </c>
+      <c r="K15" s="1">
+        <f t="shared" si="1"/>
+        <v>20.771293795591507</v>
+      </c>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1">
+        <v>241600</v>
+      </c>
+      <c r="N15" s="1">
+        <f t="shared" si="2"/>
+        <v>15.516411116170586</v>
+      </c>
+      <c r="O15" s="1"/>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B16" s="30">
+        <v>14</v>
+      </c>
+      <c r="C16" s="35">
+        <v>5.0283071801380101</v>
+      </c>
+      <c r="D16" s="33">
+        <v>7840.1029685888097</v>
+      </c>
+      <c r="E16" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <v>65875</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="0"/>
+        <v>19.573192387510147</v>
+      </c>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1">
+        <v>130700</v>
+      </c>
+      <c r="K16" s="1">
+        <f t="shared" si="1"/>
+        <v>21.891187332393717</v>
+      </c>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1">
+        <v>261400</v>
+      </c>
+      <c r="N16" s="1">
+        <f t="shared" si="2"/>
+        <v>16.352985317776341</v>
+      </c>
+      <c r="O16" s="1"/>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B17" s="30">
+        <v>15</v>
+      </c>
+      <c r="C17" s="35">
+        <v>5.5270838162584504</v>
+      </c>
+      <c r="D17" s="33">
+        <v>7840.1029685888097</v>
+      </c>
+      <c r="E17" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>70750</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="0"/>
+        <v>20.527317933009261</v>
+      </c>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1">
+        <v>140600</v>
+      </c>
+      <c r="K17" s="1">
+        <f t="shared" si="1"/>
+        <v>22.983128196861092</v>
+      </c>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1">
+        <v>281200</v>
+      </c>
+      <c r="N17" s="1">
+        <f t="shared" si="2"/>
+        <v>17.168678530455193</v>
+      </c>
+      <c r="O17" s="1"/>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B18" s="30">
+        <v>16</v>
+      </c>
+      <c r="C18" s="35">
+        <v>3.1109354170654102</v>
+      </c>
+      <c r="D18" s="33">
+        <v>10521.605614327</v>
+      </c>
+      <c r="E18" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <v>75625</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="0"/>
+        <v>21.459758873047885</v>
+      </c>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1">
+        <v>150500</v>
+      </c>
+      <c r="K18" s="1">
+        <f t="shared" si="1"/>
+        <v>24.049714530031874</v>
+      </c>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1">
+        <v>301000</v>
+      </c>
+      <c r="N18" s="1">
+        <f t="shared" si="2"/>
+        <v>17.965431597415286</v>
+      </c>
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B19" s="30">
+        <v>17</v>
+      </c>
+      <c r="C19" s="35">
+        <v>3.9839690488678698</v>
+      </c>
+      <c r="D19" s="33">
+        <v>9963.7474945948306</v>
+      </c>
+      <c r="E19" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <v>80500</v>
+      </c>
+      <c r="H19" s="1">
+        <f t="shared" si="0"/>
+        <v>22.372361745881438</v>
+      </c>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1">
+        <v>160400</v>
+      </c>
+      <c r="K19" s="1">
+        <f t="shared" si="1"/>
+        <v>25.093149170225455</v>
+      </c>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1">
+        <v>320800</v>
+      </c>
+      <c r="N19" s="1">
+        <f t="shared" si="2"/>
+        <v>18.744890065887461</v>
+      </c>
+      <c r="O19" s="1"/>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B20" s="30">
+        <v>18</v>
+      </c>
+      <c r="C20" s="35">
+        <v>6.53380060500265</v>
+      </c>
+      <c r="D20" s="33">
+        <v>12122.612259240301</v>
+      </c>
+      <c r="E20" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <v>85375</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" si="0"/>
+        <v>23.266714308031634</v>
+      </c>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1">
+        <v>170300</v>
+      </c>
+      <c r="K20" s="1">
+        <f t="shared" si="1"/>
+        <v>26.115320356229613</v>
+      </c>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1">
+        <v>340600</v>
+      </c>
+      <c r="N20" s="1">
+        <f t="shared" si="2"/>
+        <v>19.508464473395502</v>
+      </c>
+      <c r="O20" s="1"/>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B21" s="30">
+        <v>19</v>
+      </c>
+      <c r="C21" s="35">
+        <v>7.39398145593064</v>
+      </c>
+      <c r="D21" s="33">
+        <v>12941.582395224001</v>
+      </c>
+      <c r="E21" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1">
+        <v>90250</v>
+      </c>
+      <c r="H21" s="1">
+        <f t="shared" si="0"/>
+        <v>24.144194430252892</v>
+      </c>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1">
+        <v>180200</v>
+      </c>
+      <c r="K21" s="1">
+        <f t="shared" si="1"/>
+        <v>27.117862238512657</v>
+      </c>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1">
+        <v>360400</v>
+      </c>
+      <c r="N21" s="1">
+        <f t="shared" si="2"/>
+        <v>20.257375550373517</v>
+      </c>
+      <c r="O21" s="1"/>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B22" s="30">
+        <v>20</v>
+      </c>
+      <c r="C22" s="35">
+        <v>8.1867619856537406</v>
+      </c>
+      <c r="D22" s="33">
+        <v>13371.587337421901</v>
+      </c>
+      <c r="E22" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1">
+        <v>95125</v>
+      </c>
+      <c r="H22" s="1">
+        <f t="shared" si="0"/>
+        <v>25.006007622889708</v>
+      </c>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1">
+        <v>190100</v>
+      </c>
+      <c r="K22" s="1">
+        <f t="shared" si="1"/>
+        <v>28.102201079362764</v>
+      </c>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1">
+        <v>380200</v>
+      </c>
+      <c r="N22" s="1">
+        <f t="shared" si="2"/>
+        <v>20.992688732236388</v>
+      </c>
+      <c r="O22" s="1"/>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B23" s="30">
+        <v>21</v>
+      </c>
+      <c r="C23" s="35">
+        <v>8.8045616937983695</v>
+      </c>
+      <c r="D23" s="33">
+        <v>12941.582395224001</v>
+      </c>
+      <c r="E23" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G23" s="1">
+        <v>100000</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" si="0"/>
+        <v>25.853216280382611</v>
+      </c>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1">
+        <v>200000</v>
+      </c>
+      <c r="K23" s="1">
+        <f t="shared" si="1"/>
+        <v>29.069591093503838</v>
+      </c>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1">
+        <v>400000</v>
+      </c>
+      <c r="N23" s="1">
+        <f t="shared" si="2"/>
+        <v>21.715340932759247</v>
+      </c>
+      <c r="O23" s="1"/>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B24" s="30">
+        <v>22</v>
+      </c>
+      <c r="C24" s="35">
+        <v>5.44724533003233</v>
+      </c>
+      <c r="D24" s="33">
+        <v>16627.240910203102</v>
+      </c>
+      <c r="E24" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B25" s="30">
+        <v>23</v>
+      </c>
+      <c r="C25" s="35">
+        <v>5.6490409575756901</v>
+      </c>
+      <c r="D25" s="33">
+        <v>16092.5403106346</v>
+      </c>
+      <c r="E25" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B26" s="30">
+        <v>24</v>
+      </c>
+      <c r="C26" s="35">
+        <v>6.4864387144298199</v>
+      </c>
+      <c r="D26" s="33">
+        <v>17367.912964078601</v>
+      </c>
+      <c r="E26" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B27" s="30">
+        <v>25</v>
+      </c>
+      <c r="C27" s="35">
+        <v>6.4394201383862004</v>
+      </c>
+      <c r="D27" s="33">
+        <v>23055.578575730498</v>
+      </c>
+      <c r="E27" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B28" s="30">
+        <v>26</v>
+      </c>
+      <c r="C28" s="35">
+        <v>8.7407396225885297</v>
+      </c>
+      <c r="D28" s="33">
+        <v>18949.7080627377</v>
+      </c>
+      <c r="E28" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B29" s="30">
+        <v>27</v>
+      </c>
+      <c r="C29" s="35">
+        <v>8.6773801816509408</v>
+      </c>
+      <c r="D29" s="33">
+        <v>22558.6082726038</v>
+      </c>
+      <c r="E29" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B30" s="30">
+        <v>28</v>
+      </c>
+      <c r="C30" s="35">
+        <v>9.9636903277546605</v>
+      </c>
+      <c r="D30" s="33">
+        <v>21362.545308830198</v>
+      </c>
+      <c r="E30" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B31" s="30">
+        <v>29</v>
+      </c>
+      <c r="C31" s="35">
+        <v>15.083947351828099</v>
+      </c>
+      <c r="D31" s="33">
+        <v>30274.191602250699</v>
+      </c>
+      <c r="E31" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B32" s="30">
+        <v>30</v>
+      </c>
+      <c r="C32" s="35">
+        <v>11.951135288991299</v>
+      </c>
+      <c r="D32" s="33">
+        <v>41978.642582492401</v>
+      </c>
+      <c r="E32" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B33" s="30">
+        <v>31</v>
+      </c>
+      <c r="C33" s="35">
+        <v>14.7583000229055</v>
+      </c>
+      <c r="D33" s="33">
+        <v>45801.877488303398</v>
+      </c>
+      <c r="E33" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B34" s="30">
+        <v>32</v>
+      </c>
+      <c r="C34" s="35">
+        <v>15.756957145976999</v>
+      </c>
+      <c r="D34" s="33">
+        <v>41978.642582492401</v>
+      </c>
+      <c r="E34" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B35" s="30">
+        <v>33</v>
+      </c>
+      <c r="C35" s="35">
+        <v>16.823190890198099</v>
+      </c>
+      <c r="D35" s="33">
+        <v>46810.901301477803</v>
+      </c>
+      <c r="E35" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B36" s="30">
+        <v>34</v>
+      </c>
+      <c r="C36" s="35">
+        <v>18.899977859593498</v>
+      </c>
+      <c r="D36" s="33">
+        <v>46303.640964046703</v>
+      </c>
+      <c r="E36" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B37" s="37">
+        <v>35</v>
+      </c>
+      <c r="C37" s="38">
+        <v>17.1944007970875</v>
+      </c>
+      <c r="D37" s="36">
+        <v>62140.593137999102</v>
+      </c>
+      <c r="E37" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C39" s="31"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C40" s="31"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C41" s="31"/>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C42" s="31"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C43" s="31"/>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C44" s="31"/>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C45" s="31"/>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C46" s="31"/>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C47" s="31"/>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C48" s="31"/>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C49" s="31"/>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C50" s="31"/>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C51" s="31"/>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C52" s="31"/>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C53" s="31"/>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C54" s="31"/>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C55" s="31"/>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C56" s="31"/>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C57" s="31"/>
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C58" s="31"/>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C59" s="31"/>
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C60" s="31"/>
+    </row>
+    <row r="61" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C61" s="31"/>
+    </row>
+    <row r="62" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C62" s="31"/>
+    </row>
+    <row r="63" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C63" s="31"/>
+    </row>
+    <row r="64" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C64" s="31"/>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C65" s="31"/>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C66" s="31"/>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C67" s="31"/>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C68" s="31"/>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C69" s="31"/>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C70" s="31"/>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C71" s="31"/>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C72" s="31"/>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C73" s="31"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E87A9AB-8488-A647-A3B9-546303E51F88}">
   <dimension ref="B2:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated flate plate drag data
</commit_message>
<xml_diff>
--- a/docs/flat_plate_drag/flat_plate_drag_data.xlsx
+++ b/docs/flat_plate_drag/flat_plate_drag_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfiyandyhr/Github_Repos/MCEVS/docs/flat_plate_drag/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FE4D78-4895-4D4B-9519-2BA82FB7B666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF08B26-1D9F-CF4A-9B86-78C04F40A736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" xr2:uid="{9B207304-6C5B-A545-A29F-FC1BAC0A7ED9}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" activeTab="1" xr2:uid="{9B207304-6C5B-A545-A29F-FC1BAC0A7ED9}"/>
   </bookViews>
   <sheets>
     <sheet name="fuselage" sheetId="1" r:id="rId1"/>
@@ -5554,8 +5554,8 @@
           </a:graphicData>
         </a:graphic>
       </xdr:graphicFrame>
-      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-        <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+        <mc:Choice Requires="a14">
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
               <xdr:cNvPr id="8" name="TextBox 7">
@@ -5747,7 +5747,7 @@
             </xdr:txBody>
           </xdr:sp>
         </mc:Choice>
-        <mc:Fallback>
+        <mc:Fallback xmlns="">
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
               <xdr:cNvPr id="8" name="TextBox 7">
@@ -5908,8 +5908,8 @@
           </a:fontRef>
         </xdr:style>
       </xdr:cxnSp>
-      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-        <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+        <mc:Choice Requires="a14">
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
               <xdr:cNvPr id="27" name="TextBox 26">
@@ -6106,7 +6106,7 @@
             </xdr:txBody>
           </xdr:sp>
         </mc:Choice>
-        <mc:Fallback>
+        <mc:Fallback xmlns="">
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
               <xdr:cNvPr id="27" name="TextBox 26">
@@ -6190,8 +6190,8 @@
           </xdr:sp>
         </mc:Fallback>
       </mc:AlternateContent>
-      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-        <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+        <mc:Choice Requires="a14">
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
               <xdr:cNvPr id="30" name="TextBox 29">
@@ -6388,7 +6388,7 @@
             </xdr:txBody>
           </xdr:sp>
         </mc:Choice>
-        <mc:Fallback>
+        <mc:Fallback xmlns="">
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
               <xdr:cNvPr id="30" name="TextBox 29">
@@ -6472,8 +6472,8 @@
           </xdr:sp>
         </mc:Fallback>
       </mc:AlternateContent>
-      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-        <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+        <mc:Choice Requires="a14">
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
               <xdr:cNvPr id="42" name="TextBox 41">
@@ -6658,7 +6658,7 @@
             </xdr:txBody>
           </xdr:sp>
         </mc:Choice>
-        <mc:Fallback>
+        <mc:Fallback xmlns="">
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
               <xdr:cNvPr id="42" name="TextBox 41">
@@ -6770,8 +6770,8 @@
           </a:fontRef>
         </xdr:style>
       </xdr:cxnSp>
-      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-        <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+        <mc:Choice Requires="a14">
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
               <xdr:cNvPr id="46" name="TextBox 45">
@@ -6976,7 +6976,7 @@
             </xdr:txBody>
           </xdr:sp>
         </mc:Choice>
-        <mc:Fallback>
+        <mc:Fallback xmlns="">
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
               <xdr:cNvPr id="46" name="TextBox 45">
@@ -8693,7 +8693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{794DF518-2B61-2646-92A6-1D07C212A41D}">
   <dimension ref="B2:Y102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E17" zoomScaleNormal="159" workbookViewId="0">
+    <sheetView topLeftCell="E17" zoomScaleNormal="159" workbookViewId="0">
       <selection activeCell="T32" sqref="T32"/>
     </sheetView>
   </sheetViews>
@@ -11743,8 +11743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FCEE61-850F-6442-B4AC-A1CE2F893CD8}">
   <dimension ref="B2:O73"/>
   <sheetViews>
-    <sheetView topLeftCell="C16" workbookViewId="0">
-      <selection activeCell="R44" sqref="R44"/>
+    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>